<commit_message>
change GSTR 2B Default Format file
</commit_message>
<xml_diff>
--- a/dev/database/other-assets/gstr-2b-analyzer/GSTR 2B Default Format.xlsx
+++ b/dev/database/other-assets/gstr-2b-analyzer/GSTR 2B Default Format.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Goods and Services Tax  - GSTR-2B</t>
   </si>
@@ -64,15 +64,6 @@
   </si>
   <si>
     <t>Applicable % of Tax Rate</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>IRN</t>
-  </si>
-  <si>
-    <t>IRN Date</t>
   </si>
   <si>
     <t>Invoice number</t>
@@ -151,7 +142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -174,11 +165,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -218,11 +326,50 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -520,105 +667,105 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="14.4" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+    </row>
+    <row r="2" spans="1:22" ht="14.4" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+    </row>
+    <row r="3" spans="1:22" ht="14.4" customHeight="1">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+    </row>
+    <row r="4" spans="1:22" ht="14.4" customHeight="1">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="14" t="s">
@@ -666,55 +813,49 @@
       <c r="S5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="U5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="V5" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
     </row>
     <row r="6" spans="1:22" ht="36" customHeight="1">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="2"/>
@@ -1083,8 +1224,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:V3"/>
-    <mergeCell ref="A4:V4"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="A5:A6"/>
@@ -1099,8 +1242,6 @@
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="S5:S6"/>
     <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>